<commit_message>
tried to fix BOM and PaP for JLCPCB
</commit_message>
<xml_diff>
--- a/cam/Uno_v1.0_2020-11-01-BOM.xlsx
+++ b/cam/Uno_v1.0_2020-11-01-BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AG\Documents\EAGLE\projects\Uno\cam\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D408575F-E377-4CA7-AD23-FED6C8B79C5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30818D92-AD16-4F93-9E64-80CFDE48BF5F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18740" yWindow="0" windowWidth="22180" windowHeight="20940" xr2:uid="{0C47F62E-93AD-4038-96AB-D6C8EFD49D8B}"/>
+    <workbookView xWindow="380" yWindow="60" windowWidth="22180" windowHeight="20940" xr2:uid="{0C47F62E-93AD-4038-96AB-D6C8EFD49D8B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="105">
   <si>
     <t>Qty</t>
   </si>
@@ -50,18 +50,12 @@
     <t>R4, R5</t>
   </si>
   <si>
-    <t>RESISTOR, European symbol</t>
-  </si>
-  <si>
     <t>100nF</t>
   </si>
   <si>
     <t>C4, C5, C6, C7, C8, C11, C14, C15, C16, C18, C19</t>
   </si>
   <si>
-    <t>CAPACITOR, European symbol</t>
-  </si>
-  <si>
     <t>10K</t>
   </si>
   <si>
@@ -80,9 +74,6 @@
     <t>Q1</t>
   </si>
   <si>
-    <t>Quartz Crystals (MHz) SMD:</t>
-  </si>
-  <si>
     <t>12pF</t>
   </si>
   <si>
@@ -101,9 +92,6 @@
     <t>F1, F2</t>
   </si>
   <si>
-    <t>MF-SMDF Series - PRC Resettable Fuses</t>
-  </si>
-  <si>
     <t>1K</t>
   </si>
   <si>
@@ -128,9 +116,6 @@
     <t>T2</t>
   </si>
   <si>
-    <t>N-Channel MOSFET - Generic</t>
-  </si>
-  <si>
     <t>47uF</t>
   </si>
   <si>
@@ -143,9 +128,6 @@
     <t>IC2</t>
   </si>
   <si>
-    <t>Low drop fixed and adjustable positive voltage regulators 1 A</t>
-  </si>
-  <si>
     <t>AMS1117-5.0</t>
   </si>
   <si>
@@ -158,36 +140,24 @@
     <t>T1</t>
   </si>
   <si>
-    <t>P-Channel MOSFET - Generic</t>
-  </si>
-  <si>
     <t>ATMEGA328P-AU</t>
   </si>
   <si>
     <t>U2</t>
   </si>
   <si>
-    <t>Popular 328P in QFP</t>
-  </si>
-  <si>
     <t>BLUE</t>
   </si>
   <si>
     <t>LED2, LED3</t>
   </si>
   <si>
-    <t>LED</t>
-  </si>
-  <si>
     <t>CH340G</t>
   </si>
   <si>
     <t>U1</t>
   </si>
   <si>
-    <t>A simple USB 2.0 to Serial IC.</t>
-  </si>
-  <si>
     <t>GREEN</t>
   </si>
   <si>
@@ -200,27 +170,18 @@
     <t>L1, L2</t>
   </si>
   <si>
-    <t>WE-CBA SMD EMI Suppression Ferrite Bead</t>
-  </si>
-  <si>
     <t>M7</t>
   </si>
   <si>
     <t>D1</t>
   </si>
   <si>
-    <t>WE-TVSP Power TVS Diode</t>
-  </si>
-  <si>
     <t>MCP6002T-I/SN</t>
   </si>
   <si>
     <t>IC3</t>
   </si>
   <si>
-    <t>Dual General Purpose, Low Voltage, Rail-to-Rail Output Operational Amplifiers</t>
-  </si>
-  <si>
     <t>YELLOW</t>
   </si>
   <si>
@@ -348,6 +309,48 @@
   </si>
   <si>
     <t>C7377</t>
+  </si>
+  <si>
+    <t>CL31A476MPHNNNE</t>
+  </si>
+  <si>
+    <t>CL21A106KAYNNNE</t>
+  </si>
+  <si>
+    <t>CL05B104KO5NNNC</t>
+  </si>
+  <si>
+    <t>0402CG120J500NT</t>
+  </si>
+  <si>
+    <t>19-217/GHC-YR1S2/3T</t>
+  </si>
+  <si>
+    <t>19-217/BHC-ZL1M2RY/3T</t>
+  </si>
+  <si>
+    <t>19-213/Y2C-CQ2R2L/3T(CY)</t>
+  </si>
+  <si>
+    <t>X322512MSB4SI</t>
+  </si>
+  <si>
+    <t>X322516MLB4SI</t>
+  </si>
+  <si>
+    <t>0402WGF220JTCE</t>
+  </si>
+  <si>
+    <t>0402WGF1002TCE</t>
+  </si>
+  <si>
+    <t>0402WGF1004TCE</t>
+  </si>
+  <si>
+    <t>0402WGF1003TCE</t>
+  </si>
+  <si>
+    <t>0402WGF1001TCE</t>
   </si>
 </sst>
 </file>
@@ -426,7 +429,7 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -493,18 +496,18 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{02866E0B-D63F-4513-BCFC-B44DCEC0379D}" name="Uno_v1_0_BOM" displayName="Uno_v1_0_BOM" ref="A1:F25" tableType="queryTable" totalsRowShown="0" dataDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{02866E0B-D63F-4513-BCFC-B44DCEC0379D}" name="Uno_v1_0_BOM" displayName="Uno_v1_0_BOM" ref="A1:F25" tableType="queryTable" totalsRowShown="0" dataDxfId="6">
   <autoFilter ref="A1:F25" xr:uid="{A0E5FC9B-426B-4057-88B5-34DA6001A535}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F25">
     <sortCondition ref="B1:B25"/>
   </sortState>
   <tableColumns count="6">
-    <tableColumn id="35" xr3:uid="{A8CDBF85-1A63-4EF4-9E7C-6E564C8B44C6}" uniqueName="35" name="Qty" queryTableFieldId="1" dataDxfId="6"/>
-    <tableColumn id="37" xr3:uid="{B8B3B57F-C6FD-40FF-A2AB-6F110361D393}" uniqueName="37" name="Designator" queryTableFieldId="36" dataDxfId="5"/>
-    <tableColumn id="38" xr3:uid="{0BDAA507-4770-44A4-B1D7-DD0B6EC3E0E5}" uniqueName="38" name="Footprint" queryTableFieldId="37" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{7252855D-2960-4DA4-ACD5-50B6E65A941C}" uniqueName="2" name="Comment" queryTableFieldId="2" dataDxfId="3"/>
-    <tableColumn id="39" xr3:uid="{4FE9416B-E23C-4B16-A8B3-4045365B2D45}" uniqueName="39" name="LCSC Part #" queryTableFieldId="38" dataDxfId="2"/>
-    <tableColumn id="6" xr3:uid="{77DA19C9-97CF-4D3B-8778-9C0A010FBC8F}" uniqueName="6" name="Description" queryTableFieldId="6" dataDxfId="1"/>
+    <tableColumn id="35" xr3:uid="{A8CDBF85-1A63-4EF4-9E7C-6E564C8B44C6}" uniqueName="35" name="Qty" queryTableFieldId="1" dataDxfId="5"/>
+    <tableColumn id="37" xr3:uid="{B8B3B57F-C6FD-40FF-A2AB-6F110361D393}" uniqueName="37" name="Designator" queryTableFieldId="36" dataDxfId="4"/>
+    <tableColumn id="38" xr3:uid="{0BDAA507-4770-44A4-B1D7-DD0B6EC3E0E5}" uniqueName="38" name="Footprint" queryTableFieldId="37" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{7252855D-2960-4DA4-ACD5-50B6E65A941C}" uniqueName="2" name="Comment" queryTableFieldId="2" dataDxfId="2"/>
+    <tableColumn id="39" xr3:uid="{4FE9416B-E23C-4B16-A8B3-4045365B2D45}" uniqueName="39" name="LCSC Part #" queryTableFieldId="38" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{77DA19C9-97CF-4D3B-8778-9C0A010FBC8F}" uniqueName="6" name="Description" queryTableFieldId="6" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -809,7 +812,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E81F28A-B995-4967-A574-8F073559577A}">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
@@ -830,499 +833,499 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="1">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F2" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="1">
+        <v>11</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F5" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A7" s="1">
+        <v>2</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A9" s="1">
+        <v>1</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>1</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="F10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A11" s="1">
+        <v>2</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A12" s="1">
+        <v>1</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A13" s="1">
+        <v>2</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F13" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A14" s="1">
+        <v>1</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F14" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A15" s="1">
+        <v>1</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A16" s="1">
+        <v>1</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E16" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A2" s="3">
-        <v>3</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="F16" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17" s="1">
+        <v>2</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F17" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A18" s="1">
+        <v>1</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A3" s="3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A4" s="3">
-        <v>11</v>
-      </c>
-      <c r="B4" s="3" t="s">
+      <c r="C18" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D18" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A5" s="3">
-        <v>4</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A6" s="3">
-        <v>1</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="D6" s="3" t="s">
+      <c r="E18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A19" s="1">
+        <v>2</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A7" s="3">
-        <v>2</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A8" s="3">
-        <v>1</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A9" s="3">
-        <v>1</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A10" s="3">
-        <v>1</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="E19" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F19" t="s">
         <v>102</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A11" s="3">
-        <v>2</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A12" s="3">
-        <v>1</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A13" s="3">
-        <v>2</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A14" s="3">
-        <v>1</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A15" s="3">
-        <v>1</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A16" s="3">
-        <v>1</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="F16" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A17" s="3">
-        <v>2</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A18" s="3">
-        <v>1</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A19" s="3">
-        <v>2</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E19" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="F19" s="3" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A20" s="3">
+      <c r="A20" s="1">
         <v>2</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F20" s="3" t="s">
-        <v>4</v>
+        <v>54</v>
+      </c>
+      <c r="F20" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A21" s="3">
+      <c r="A21" s="1">
         <v>5</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E21" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F21" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22" s="1">
+        <v>1</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23" s="1">
+        <v>1</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24" s="1">
+        <v>1</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25" s="1">
+        <v>1</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="E25" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="F21" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A22" s="3">
-        <v>1</v>
-      </c>
-      <c r="B22" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D22" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="F22" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A23" s="3">
-        <v>1</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D23" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E23" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="F23" s="3" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A24" s="3">
-        <v>1</v>
-      </c>
-      <c r="B24" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D24" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="E24" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="F24" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A25" s="3">
-        <v>1</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>43</v>
+      <c r="F25" t="s">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>